<commit_message>
work on landings data
</commit_message>
<xml_diff>
--- a/data/landings/swfsc/species_key/long_list_key_v2.xlsx
+++ b/data/landings/swfsc/species_key/long_list_key_v2.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/swfsc/species_key/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8A9AA594-1DE6-2349-8660-98F57C77ACBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162755A4-F8EC-A147-BD6D-4384D662D72C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13540" yWindow="660" windowWidth="21540" windowHeight="25980"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="21540" windowHeight="25980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="long_list_key_v1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="688">
   <si>
     <t>comm_name_orig</t>
   </si>
@@ -1985,12 +1985,114 @@
   </si>
   <si>
     <t>Pogonichthys macrolepidotus</t>
+  </si>
+  <si>
+    <t>Eptatretus spp.</t>
+  </si>
+  <si>
+    <t>Sebastes spp. (blue/black)</t>
+  </si>
+  <si>
+    <t>Sebastes spp. (bocaccio/chilipeppe)</t>
+  </si>
+  <si>
+    <t>Sebastes spp. (canary/vermillion)</t>
+  </si>
+  <si>
+    <t>Sebastes spp. (deep red)</t>
+  </si>
+  <si>
+    <t>Sebastes spp. (small red)</t>
+  </si>
+  <si>
+    <t>Sebastes spp. (canary)</t>
+  </si>
+  <si>
+    <t>Sebastes spp. (nearshore)</t>
+  </si>
+  <si>
+    <t>Sebastes spp. (shelf)</t>
+  </si>
+  <si>
+    <t>Sebastes spp. (slope)</t>
+  </si>
+  <si>
+    <t>Selachii spp.</t>
+  </si>
+  <si>
+    <t>Lutianidae spp.</t>
+  </si>
+  <si>
+    <t>Polyplacophora spp.</t>
+  </si>
+  <si>
+    <t>Sciaenidae spp.</t>
+  </si>
+  <si>
+    <t>Holothuroidea spp.</t>
+  </si>
+  <si>
+    <t>Pleuronectidae spp.</t>
+  </si>
+  <si>
+    <t>Rajiformes spp.</t>
+  </si>
+  <si>
+    <t>Rajidae spp.</t>
+  </si>
+  <si>
+    <t>Pleuronectiformes spp.</t>
+  </si>
+  <si>
+    <t>Osteichthyes spp.</t>
+  </si>
+  <si>
+    <t>Carangidae spp.</t>
+  </si>
+  <si>
+    <t>Echinodermata spp.</t>
+  </si>
+  <si>
+    <t>Echinoidea spp.</t>
+  </si>
+  <si>
+    <t>Gastropoda spp.</t>
+  </si>
+  <si>
+    <t>Aplysia spp.</t>
+  </si>
+  <si>
+    <t>Chelonioidea spp.</t>
+  </si>
+  <si>
+    <t>Testudines spp.</t>
+  </si>
+  <si>
+    <t>Pandalus platyceros</t>
+  </si>
+  <si>
+    <t>Decapoda spp.</t>
+  </si>
+  <si>
+    <t>Crayfish spp.</t>
+  </si>
+  <si>
+    <t>Anura spp.</t>
+  </si>
+  <si>
+    <t>Percidae spp.</t>
+  </si>
+  <si>
+    <t>Leukoma staminea</t>
+  </si>
+  <si>
+    <t>Farfantepenaeus californiensis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2824,11 +2926,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3530,7 +3632,7 @@
         <v>469</v>
       </c>
       <c r="B50" t="s">
-        <v>63</v>
+        <v>665</v>
       </c>
       <c r="C50" t="s">
         <v>22</v>
@@ -3543,6 +3645,9 @@
       <c r="A51" t="s">
         <v>53</v>
       </c>
+      <c r="B51" t="s">
+        <v>666</v>
+      </c>
       <c r="C51" t="s">
         <v>22</v>
       </c>
@@ -3554,6 +3659,9 @@
       <c r="A52" t="s">
         <v>99</v>
       </c>
+      <c r="B52" t="s">
+        <v>683</v>
+      </c>
       <c r="C52" t="s">
         <v>22</v>
       </c>
@@ -3565,6 +3673,9 @@
       <c r="A53" t="s">
         <v>102</v>
       </c>
+      <c r="B53" t="s">
+        <v>667</v>
+      </c>
       <c r="C53" t="s">
         <v>22</v>
       </c>
@@ -3576,6 +3687,9 @@
       <c r="A54" t="s">
         <v>109</v>
       </c>
+      <c r="B54" t="s">
+        <v>668</v>
+      </c>
       <c r="C54" t="s">
         <v>22</v>
       </c>
@@ -3587,6 +3701,9 @@
       <c r="A55" t="s">
         <v>125</v>
       </c>
+      <c r="B55" t="s">
+        <v>669</v>
+      </c>
       <c r="C55" t="s">
         <v>22</v>
       </c>
@@ -3598,6 +3715,9 @@
       <c r="A56" t="s">
         <v>128</v>
       </c>
+      <c r="B56" t="s">
+        <v>684</v>
+      </c>
       <c r="C56" t="s">
         <v>22</v>
       </c>
@@ -3609,6 +3729,9 @@
       <c r="A57" t="s">
         <v>146</v>
       </c>
+      <c r="B57" t="s">
+        <v>654</v>
+      </c>
       <c r="C57" t="s">
         <v>22</v>
       </c>
@@ -3620,6 +3743,9 @@
       <c r="A58" t="s">
         <v>284</v>
       </c>
+      <c r="B58" t="s">
+        <v>655</v>
+      </c>
       <c r="C58" t="s">
         <v>22</v>
       </c>
@@ -3631,6 +3757,9 @@
       <c r="A59" t="s">
         <v>285</v>
       </c>
+      <c r="B59" t="s">
+        <v>656</v>
+      </c>
       <c r="C59" t="s">
         <v>22</v>
       </c>
@@ -3642,6 +3771,9 @@
       <c r="A60" t="s">
         <v>288</v>
       </c>
+      <c r="B60" t="s">
+        <v>657</v>
+      </c>
       <c r="C60" t="s">
         <v>22</v>
       </c>
@@ -3653,6 +3785,9 @@
       <c r="A61" t="s">
         <v>289</v>
       </c>
+      <c r="B61" t="s">
+        <v>658</v>
+      </c>
       <c r="C61" t="s">
         <v>22</v>
       </c>
@@ -3664,6 +3799,9 @@
       <c r="A62" t="s">
         <v>296</v>
       </c>
+      <c r="B62" t="s">
+        <v>659</v>
+      </c>
       <c r="C62" t="s">
         <v>22</v>
       </c>
@@ -3675,6 +3813,9 @@
       <c r="A63" t="s">
         <v>303</v>
       </c>
+      <c r="B63" t="s">
+        <v>660</v>
+      </c>
       <c r="C63" t="s">
         <v>22</v>
       </c>
@@ -3686,6 +3827,9 @@
       <c r="A64" t="s">
         <v>336</v>
       </c>
+      <c r="B64" t="s">
+        <v>661</v>
+      </c>
       <c r="C64" t="s">
         <v>22</v>
       </c>
@@ -3697,6 +3841,9 @@
       <c r="A65" t="s">
         <v>337</v>
       </c>
+      <c r="B65" t="s">
+        <v>662</v>
+      </c>
       <c r="C65" t="s">
         <v>22</v>
       </c>
@@ -3708,6 +3855,9 @@
       <c r="A66" t="s">
         <v>338</v>
       </c>
+      <c r="B66" t="s">
+        <v>663</v>
+      </c>
       <c r="C66" t="s">
         <v>22</v>
       </c>
@@ -3719,6 +3869,9 @@
       <c r="A67" t="s">
         <v>570</v>
       </c>
+      <c r="B67" t="s">
+        <v>676</v>
+      </c>
       <c r="C67" t="s">
         <v>22</v>
       </c>
@@ -3730,6 +3883,9 @@
       <c r="A68" t="s">
         <v>573</v>
       </c>
+      <c r="B68" t="s">
+        <v>677</v>
+      </c>
       <c r="C68" t="s">
         <v>22</v>
       </c>
@@ -3741,6 +3897,9 @@
       <c r="A69" t="s">
         <v>235</v>
       </c>
+      <c r="B69" t="s">
+        <v>670</v>
+      </c>
       <c r="C69" t="s">
         <v>22</v>
       </c>
@@ -3752,6 +3911,9 @@
       <c r="A70" t="s">
         <v>381</v>
       </c>
+      <c r="B70" t="s">
+        <v>678</v>
+      </c>
       <c r="C70" t="s">
         <v>22</v>
       </c>
@@ -3763,6 +3925,9 @@
       <c r="A71" t="s">
         <v>394</v>
       </c>
+      <c r="B71" t="s">
+        <v>664</v>
+      </c>
       <c r="C71" t="s">
         <v>22</v>
       </c>
@@ -3774,6 +3939,9 @@
       <c r="A72" t="s">
         <v>450</v>
       </c>
+      <c r="B72" t="s">
+        <v>671</v>
+      </c>
       <c r="C72" t="s">
         <v>22</v>
       </c>
@@ -3785,6 +3953,9 @@
       <c r="A73" t="s">
         <v>493</v>
       </c>
+      <c r="B73" t="s">
+        <v>672</v>
+      </c>
       <c r="C73" t="s">
         <v>22</v>
       </c>
@@ -3796,6 +3967,9 @@
       <c r="A74" t="s">
         <v>561</v>
       </c>
+      <c r="B74" t="s">
+        <v>669</v>
+      </c>
       <c r="C74" t="s">
         <v>22</v>
       </c>
@@ -3807,6 +3981,9 @@
       <c r="A75" t="s">
         <v>562</v>
       </c>
+      <c r="B75" t="s">
+        <v>680</v>
+      </c>
       <c r="C75" t="s">
         <v>22</v>
       </c>
@@ -3818,6 +3995,9 @@
       <c r="A76" t="s">
         <v>563</v>
       </c>
+      <c r="B76" t="s">
+        <v>679</v>
+      </c>
       <c r="C76" t="s">
         <v>22</v>
       </c>
@@ -3829,6 +4009,9 @@
       <c r="A77" t="s">
         <v>564</v>
       </c>
+      <c r="B77" t="s">
+        <v>673</v>
+      </c>
       <c r="C77" t="s">
         <v>22</v>
       </c>
@@ -3840,6 +4023,9 @@
       <c r="A78" t="s">
         <v>565</v>
       </c>
+      <c r="B78" t="s">
+        <v>673</v>
+      </c>
       <c r="C78" t="s">
         <v>22</v>
       </c>
@@ -3851,8 +4037,11 @@
       <c r="A79" t="s">
         <v>59</v>
       </c>
+      <c r="B79" t="s">
+        <v>686</v>
+      </c>
       <c r="C79" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D79" t="s">
         <v>7</v>
@@ -3862,6 +4051,9 @@
       <c r="A80" t="s">
         <v>112</v>
       </c>
+      <c r="B80" t="s">
+        <v>675</v>
+      </c>
       <c r="C80" t="s">
         <v>22</v>
       </c>
@@ -3873,6 +4065,9 @@
       <c r="A81" t="s">
         <v>168</v>
       </c>
+      <c r="B81" t="s">
+        <v>674</v>
+      </c>
       <c r="C81" t="s">
         <v>22</v>
       </c>
@@ -3884,6 +4079,9 @@
       <c r="A82" t="s">
         <v>222</v>
       </c>
+      <c r="B82" t="s">
+        <v>685</v>
+      </c>
       <c r="C82" t="s">
         <v>22</v>
       </c>
@@ -3895,6 +4093,9 @@
       <c r="A83" t="s">
         <v>231</v>
       </c>
+      <c r="B83" t="s">
+        <v>682</v>
+      </c>
       <c r="C83" t="s">
         <v>22</v>
       </c>
@@ -6791,7 +6992,7 @@
         <v>230</v>
       </c>
       <c r="B290" t="s">
-        <v>605</v>
+        <v>681</v>
       </c>
       <c r="C290" t="s">
         <v>6</v>
@@ -7449,7 +7650,7 @@
         <v>227</v>
       </c>
       <c r="B337" t="s">
-        <v>63</v>
+        <v>687</v>
       </c>
       <c r="C337" t="s">
         <v>6</v>
@@ -7529,11 +7730,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D342">
-    <sortState ref="A2:D342">
-      <sortCondition ref="C1:C342"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:D342" xr:uid="{E6E038A2-3575-CE44-BB17-5C4DC9F10E4C}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>